<commit_message>
Handle footnotes during xlsx export
This commit implements handling of tables that contains footnotes and/or reference symbols so that they are properly exported to xlsx.
Also made the effort the clean up the code a bit.
</commit_message>
<xml_diff>
--- a/tests/testthat/_snaps/xlsx_export/Table_8.xlsx
+++ b/tests/testthat/_snaps/xlsx_export/Table_8.xlsx
@@ -6,7 +6,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -1458,7 +1458,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" ht="27" customHeight="1">
+    <row r="39">
       <c r="A39" s="6" t="s">
         <v>7</v>
       </c>

</xml_diff>